<commit_message>
Update exercices_gini_afc2022 (version 1).xlsx
</commit_message>
<xml_diff>
--- a/exercices/exercices_gini_afc2022 (version 1).xlsx
+++ b/exercices/exercices_gini_afc2022 (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gueney\Documents\GitHub\les-mesures-de-l-conomie\exercices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1D98AC-F8E8-4578-9671-8685573E6842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22352609-0516-448B-BB79-4D3B317E3FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{0A857FEE-5B62-478B-B26F-1439DD0DBBE3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>seuil inférieur du groupe</t>
   </si>
@@ -221,9 +221,6 @@
     <t>a = b/(b-1)</t>
   </si>
   <si>
-    <t>k=s*p^(1/a)</t>
-  </si>
-  <si>
     <t>total I top group</t>
   </si>
   <si>
@@ -233,10 +230,32 @@
     <t>Part du 1%: interpolation de Pareto</t>
   </si>
   <si>
-    <t>y_bar</t>
+    <t>Part du 10%</t>
   </si>
   <si>
-    <t>Part du 10%</t>
+    <t>parametre b</t>
+  </si>
+  <si>
+    <t>coefficient de pareto</t>
+  </si>
+  <si>
+    <t>revenu moyen au dessus de p</t>
+  </si>
+  <si>
+    <t>seuil de revenu pour appartenir au percentile p</t>
+  </si>
+  <si>
+    <t>parametre k</t>
+  </si>
+  <si>
+    <t>y_bar = a/(a-1)*s</t>
+  </si>
+  <si>
+    <t>Revenu moyen au dessus du seuil</t>
+  </si>
+  <si>
+    <t>k=s*p^(1/a)
+p = share of units with income larger than s</t>
   </si>
 </sst>
 </file>
@@ -3525,16 +3544,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>760412</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1725612</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523873</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>180973</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1050923</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>123823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5643,8 +5662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988134C0-BA93-4AA9-AB60-815506C21888}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5652,8 +5671,12 @@
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="70.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -7315,7 +7338,7 @@
         <v>0.21471904349262805</v>
       </c>
       <c r="N33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O33" s="32">
         <f>O23+((O22-O23)*(0.1-M23))/(M22-M23)</f>
@@ -7443,6 +7466,13 @@
         <f t="shared" si="7"/>
         <v>-0.40271968167192423</v>
       </c>
+      <c r="F49" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
@@ -7453,15 +7483,26 @@
         <f t="shared" si="7"/>
         <v>-0.44523318400886275</v>
       </c>
-      <c r="F50" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" t="s">
+        <v>67</v>
+      </c>
+      <c r="J50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="6"/>
         <v>4.8294456902556702</v>
@@ -7471,7 +7512,7 @@
         <v>-0.48873371805696725</v>
       </c>
       <c r="E51" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F51" t="s">
         <v>58</v>
@@ -7479,14 +7520,14 @@
       <c r="G51" t="s">
         <v>59</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I51" t="s">
+        <v>61</v>
+      </c>
+      <c r="J51" t="s">
         <v>60</v>
-      </c>
-      <c r="I51" t="s">
-        <v>62</v>
-      </c>
-      <c r="J51" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -7511,16 +7552,16 @@
         <v>2.0152028146280223</v>
       </c>
       <c r="H52">
-        <f>A25*((D25/D30)^(1/G52))</f>
-        <v>25661.083744426138</v>
+        <f>A25*(SUM(D25:D29)/D30)^(1/G52)</f>
+        <v>36276.764969976786</v>
       </c>
       <c r="I52">
         <f>H52/(0.01^(1/G52))</f>
-        <v>252191.78301239229</v>
+        <v>356520.48568241531</v>
       </c>
       <c r="J52">
         <f>I52*F52*0.01*D32</f>
-        <v>1254345819.7927201</v>
+        <v>1773253575.2928684</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -7534,7 +7575,7 @@
       </c>
       <c r="J53">
         <f>J52/C30</f>
-        <v>7.7839347346944823E-2</v>
+        <v>0.11004054767308313</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -7928,7 +7969,7 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:Q1"/>
     <mergeCell ref="B69:C69"/>
-    <mergeCell ref="F50:J50"/>
+    <mergeCell ref="F49:J49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>